<commit_message>
mise a jour des donnees vrai 05-07-2021
</commit_message>
<xml_diff>
--- a/complaints_call/storage_xlsx/dataset_call.xlsx
+++ b/complaints_call/storage_xlsx/dataset_call.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="600" windowWidth="24000" windowHeight="9585" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9585" windowWidth="24000" xWindow="0" yWindow="600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -43,15 +43,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U16"/>
+  <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="U1" sqref="U1"/>
@@ -2136,7 +2136,970 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>624042702533402</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>237669800046</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>isActiveIMSI:Subscriber is not attached. Try to restart phone;</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>624042732168871</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>237664022676</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>3566780923618278</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>237660002052</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>10.124.148.4</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>160664022676</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>160664022676</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>160664022676</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>KNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>DOMS02:KNOWN SUBSCRIBER;cfb:cfb is defined to 160664022676;cfnrc:cfnrc is defined to 160664022676;cfnry:cfnry is defined to 160664022676;</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>624042732168871</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>237664022676</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>3566780923618278</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>237660002052</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>10.124.148.4</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>160664022676</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>160664022676</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>160664022676</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>KNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>odboc:Barring oc in HLR;DOMS02:KNOWN SUBSCRIBER;cfb:cfb is defined to 160664022676;cfnrc:cfnrc is defined to 160664022676;cfnry:cfnry is defined to 160664022676;</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>624042732168871</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>237664022676</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>3566780923618278</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>237660002052</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>10.124.148.4</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>160664022676</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>160664022676</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>160664022676</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>KNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>odboc:Barring oc in HLR;DOMS02:KNOWN SUBSCRIBER;cfb:cfb is defined to 160664022676;cfnrc:cfnrc is defined to 160664022676;cfnry:cfnry is defined to 160664022676;</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>624042732168871</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>237664022676</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>3566780923618278</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>237660002052</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>10.124.148.4</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>160664022676</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>16066022676</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>160664022676</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>KNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>DOMS02:KNOWN SUBSCRIBER;cfb:cfb is defined to 160664022676;cfnrc:cfnrc is defined to 16066022676;cfnry:cfnry is defined to 160664022676;</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>624042732168871</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>237664022676</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>3566780923618278</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>237660002052</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>10.124.148.4</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>160664022676</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>16066022676</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>160664022676</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>KNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>DOMS02:KNOWN SUBSCRIBER;cfb:cfb is defined to 160664022676;cfnrc:cfnrc is defined to 16066022676;cfnry:cfnry is defined to 160664022676;</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>624042732168871</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>237664022676</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>3566780923618278</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>160664022676</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>160664022676</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>160664022676</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>no_exist:Subscriber exists in any MSS. Restart phone;cfb:cfb is defined to 160664022676;cfnrc:cfnrc is defined to 160664022676;cfnry:cfnry is defined to 160664022676;</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>624042700253500</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>237661341827</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>8655500200407700</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>237660001052</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>10.124.208.81</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>no_exist:Subscriber exists in any MSS. Restart phone;result:Everything is ok in HLR;</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>624042702533402</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>237669800046</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>isActiveIMSI:Subscriber is not attached. Try to restart phone;</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
derniere mise a jour - 07/07/2021 RobIC
</commit_message>
<xml_diff>
--- a/complaints_call/storage_xlsx/dataset_call.xlsx
+++ b/complaints_call/storage_xlsx/dataset_call.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="600" windowWidth="24000" windowHeight="9585" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9585" windowWidth="24000" xWindow="0" yWindow="600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -43,15 +43,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U42"/>
+  <dimension ref="A1:U55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="U1" sqref="U1"/>
@@ -4918,7 +4918,1399 @@
         </is>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>624042747312230</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>237663744490</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>3587660809968478</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>237660002052</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>10.124.148.4</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="S43" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="T43" t="inlineStr">
+        <is>
+          <t>KNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>DOMS02:KNOWN SUBSCRIBER;result:ok;</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>624042747312230</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>237663744490</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>3587660809968478</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>237660002052</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>10.124.148.4</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="S44" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="T44" t="inlineStr">
+        <is>
+          <t>KNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="U44" t="inlineStr">
+        <is>
+          <t>DOMS02:KNOWN SUBSCRIBER;result:ok;</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>624042747827156</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>237669595858</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>8630780379935655</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>237660002051</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>10.124.140.1</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="S45" t="inlineStr">
+        <is>
+          <t>KNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="T45" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="U45" t="inlineStr">
+        <is>
+          <t>DOMS01:KNOWN SUBSCRIBER;odbic:Barring ic solved;</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>624042747827156</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>237669595858</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>8630780379935655</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>237660002051</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>10.124.140.1</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="S46" t="inlineStr">
+        <is>
+          <t>KNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="T46" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t>DOMS01:KNOWN SUBSCRIBER;odbic:Barring ic solved;</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>624042747827156</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>237669595858</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>8630780379935655</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>237660002051</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>10.124.140.1</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="S47" t="inlineStr">
+        <is>
+          <t>KNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="T47" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="U47" t="inlineStr">
+        <is>
+          <t>DOMS01:KNOWN SUBSCRIBER;result:ok;</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>624042747827156</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>237669595858</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>8630780379935655</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>237660002051</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>10.124.140.1</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="S48" t="inlineStr">
+        <is>
+          <t>KNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="T48" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="U48" t="inlineStr">
+        <is>
+          <t>DOMS01:KNOWN SUBSCRIBER;result:ok;</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>624042747827156</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>237669595858</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>8630780379935655</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>237660002051</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>10.124.140.1</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="S49" t="inlineStr">
+        <is>
+          <t>KNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="T49" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="U49" t="inlineStr">
+        <is>
+          <t>DOMS01:KNOWN SUBSCRIBER;odbic:Barring ic solved;</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>624042747827156</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>237669595858</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>8630780379935655</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>237660002051</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>10.124.140.1</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="S50" t="inlineStr">
+        <is>
+          <t>KNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="T50" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t>odboc:Barring oc solved;DOMS01:KNOWN SUBSCRIBER;odbic:Barring ic solved;</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>624042747827156</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>237669595858</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>8630780379935655</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>237660002051</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>10.124.140.1</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="S51" t="inlineStr">
+        <is>
+          <t>KNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="T51" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="U51" t="inlineStr">
+        <is>
+          <t>DOMS01:KNOWN SUBSCRIBER;result:ok;</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>624042747827156</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>237669595858</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>8630780379935655</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>237660002051</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>10.124.140.1</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="S52" t="inlineStr">
+        <is>
+          <t>KNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="T52" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="U52" t="inlineStr">
+        <is>
+          <t>odboc:Barring oc solved;DOMS01:KNOWN SUBSCRIBER;odbic:Barring ic solved;</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>624042747827156</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>237669595858</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>8630780379935655</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>237660002051</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>10.124.140.1</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P53" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="S53" t="inlineStr">
+        <is>
+          <t>KNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="T53" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="U53" t="inlineStr">
+        <is>
+          <t>DOMS01:KNOWN SUBSCRIBER;result:ok;</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>624042747827156</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>237669595858</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>8630780379935655</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>237660002051</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>10.124.140.1</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P54" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="S54" t="inlineStr">
+        <is>
+          <t>KNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="T54" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="U54" t="inlineStr">
+        <is>
+          <t>DOMS01:KNOWN SUBSCRIBER;result:ok;</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>searchResponse:requestID=ee4874dc-cedf-4198-b96e-be2e9aef8cac, errorCode=32, errorMessage= error result (32); matchedDN = dc=MSISDN,DC=C-NTDB,entries:
+END OF SEARCH ENTRIES.,</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P55" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="R55" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="S55" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="T55" t="inlineStr">
+        <is>
+          <t>UNKNOWN SUBSCRIBER</t>
+        </is>
+      </c>
+      <c r="U55" t="inlineStr">
+        <is>
+          <t>ldapResponse:Unknow Subscriber in HLR;</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>